<commit_message>
:truck: data from Carlos
</commit_message>
<xml_diff>
--- a/demo/Zhang_PAMO_selectivity_Gibbs.xlsx
+++ b/demo/Zhang_PAMO_selectivity_Gibbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteo/Coding/Epistasis_Calculator/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{492188A3-8796-7D42-BB13-6E28E93BA7C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB7C0B3-EDA9-0544-B2FE-4F428407E8ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15740" yWindow="560" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40000" yWindow="3080" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_name" sheetId="1" r:id="rId1"/>
@@ -457,7 +457,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -599,7 +599,7 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>4.8</v>
+        <v>-4.8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -619,7 +619,7 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <v>4.5999999999999996</v>
+        <v>-4.5999999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -719,7 +719,7 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>7.3</v>
+        <v>-7.3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -739,7 +739,7 @@
         <v>2</v>
       </c>
       <c r="F14">
-        <v>4.4000000000000004</v>
+        <v>-4.4000000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -779,7 +779,7 @@
         <v>2</v>
       </c>
       <c r="F16">
-        <v>4.3</v>
+        <v>-4.3</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -799,7 +799,7 @@
         <v>2</v>
       </c>
       <c r="F17">
-        <v>9.1</v>
+        <v>-9.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:truck: Carlos fixed the data
</commit_message>
<xml_diff>
--- a/demo/Zhang_PAMO_selectivity_Gibbs.xlsx
+++ b/demo/Zhang_PAMO_selectivity_Gibbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteo/Coding/Epistasis_Calculator/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB7C0B3-EDA9-0544-B2FE-4F428407E8ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C870AFF7-C072-B54D-ADBE-4AFEA72B7805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40000" yWindow="3080" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="24">
   <si>
-    <t>Replicate n°1</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>Replicate</t>
   </si>
 </sst>
 </file>
@@ -457,46 +457,46 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>7.3</v>
@@ -504,19 +504,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>11.4</v>
@@ -524,19 +524,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>4.2</v>
@@ -544,19 +544,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>4.2</v>
@@ -564,19 +564,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>10.4</v>
@@ -584,19 +584,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>-4.8</v>
@@ -604,19 +604,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>-4.5999999999999996</v>
@@ -624,19 +624,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>1.2</v>
@@ -644,19 +644,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>3</v>
@@ -664,19 +664,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>5.6</v>
@@ -684,19 +684,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>4.5999999999999996</v>
@@ -704,19 +704,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>-7.3</v>
@@ -724,19 +724,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>-4.4000000000000004</v>
@@ -744,19 +744,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>2</v>
@@ -764,19 +764,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>-4.3</v>
@@ -784,19 +784,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <v>-9.1</v>

</xml_diff>